<commit_message>
"yangi classlar qushilgan yangi step"
</commit_message>
<xml_diff>
--- a/kassirlar ro`yxati.xlsx
+++ b/kassirlar ro`yxati.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">ID raqami </t>
   </si>
@@ -32,10 +32,10 @@
     <t>Holati</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
-    <t>Ali Aliyev</t>
+    <t>ali aliyevv</t>
   </si>
   <si>
     <t>+998971234567</t>
@@ -47,19 +47,7 @@
     <t>ACCOUNTENT</t>
   </si>
   <si>
-    <t>BLOCK</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Javohir yallayev</t>
-  </si>
-  <si>
-    <t>+998971234554</t>
-  </si>
-  <si>
-    <t>321</t>
+    <t>ACTIVE</t>
   </si>
 </sst>
 </file>
@@ -104,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -150,26 +138,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>